<commit_message>
added scheduler for background report generation, added more database queries
</commit_message>
<xml_diff>
--- a/certificate_templates/demo_upload.xlsx
+++ b/certificate_templates/demo_upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Automatic-Certificate-generator\certificate_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4960F619-CE87-41E3-908C-433D1F0D4D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1175A09-2D74-4288-A57C-5F7C7374D833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6459BBA3-DF93-4035-8702-AD47AF5AF799}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>Ganshyam Gawhale</t>
+  </si>
+  <si>
+    <t>ROLL_NO</t>
+  </si>
+  <si>
+    <t>MKY1298</t>
+  </si>
+  <si>
+    <t>MKY1232</t>
+  </si>
+  <si>
+    <t>MKY1222</t>
   </si>
 </sst>
 </file>
@@ -442,125 +454,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5EBB6E-6C25-48D2-9962-A2C27002125A}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" customWidth="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" customWidth="1"/>
+    <col min="8" max="8" width="26.44140625" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed small implementation formats, against the frontend integration
</commit_message>
<xml_diff>
--- a/certificate_templates/demo_upload.xlsx
+++ b/certificate_templates/demo_upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Automatic-Certificate-generator\certificate_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1175A09-2D74-4288-A57C-5F7C7374D833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AED7744-83A0-401A-A2EF-E52893845C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6459BBA3-DF93-4035-8702-AD47AF5AF799}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6459BBA3-DF93-4035-8702-AD47AF5AF799}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,9 @@
     <t>NAME</t>
   </si>
   <si>
-    <t>FATHER_NAME</t>
-  </si>
-  <si>
     <t>COURSE</t>
   </si>
   <si>
-    <t>COURSE_ID</t>
-  </si>
-  <si>
     <t>CENTER</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>Ganshyam Gawhale</t>
   </si>
   <si>
-    <t>ROLL_NO</t>
-  </si>
-  <si>
     <t>MKY1298</t>
   </si>
   <si>
@@ -103,6 +94,15 @@
   </si>
   <si>
     <t>MKY1222</t>
+  </si>
+  <si>
+    <t>ROLL NO</t>
+  </si>
+  <si>
+    <t>FATHER NAME</t>
+  </si>
+  <si>
+    <t>COURSE ID</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,28 +478,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -507,28 +507,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -536,28 +536,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -565,28 +565,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
         <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>